<commit_message>
TISDEV-4216 add support for Rotations to people import
</commit_message>
<xml_diff>
--- a/generic-upload-service/src/test/resources/TIS Recruitment Import Template - test - single.xlsx
+++ b/generic-upload-service/src/test/resources/TIS Recruitment Import Template - test - single.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
   <si>
     <t>Forenames *</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Programme End Date</t>
   </si>
   <si>
+    <t>Rotation #1</t>
+  </si>
+  <si>
     <t>NTN (Programme)</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
   </si>
   <si>
     <t>Substantive</t>
+  </si>
+  <si>
+    <t>Trauma &amp; Orthopaedic Surgery NCEL UCLP - RNOH</t>
   </si>
   <si>
     <t>General (Internal) Medicine</t>
@@ -197,7 +203,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="10"/>
+        <color indexed="11"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>random.guy@hotmail.co.uk</t>
@@ -267,16 +273,22 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="10"/>
+      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -289,16 +301,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -315,19 +327,19 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -347,6 +359,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff0000ff"/>
     </indexedColors>
@@ -499,9 +512,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -581,7 +594,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -609,10 +622,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -868,9 +881,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1158,7 +1171,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1186,10 +1199,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1440,7 +1453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AZ10"/>
+  <dimension ref="A1:BA10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1459,7 +1472,7 @@
     <col min="11" max="11" width="10.8516" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.8516" style="1" customWidth="1"/>
     <col min="13" max="13" width="10.8516" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.8516" style="1" customWidth="1"/>
+    <col min="14" max="14" width="41.8516" style="1" customWidth="1"/>
     <col min="15" max="15" width="10.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="10.8516" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.8516" style="1" customWidth="1"/>
@@ -1474,9 +1487,9 @@
     <col min="26" max="26" width="10.8516" style="1" customWidth="1"/>
     <col min="27" max="27" width="10.8516" style="1" customWidth="1"/>
     <col min="28" max="28" width="10.8516" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.1719" style="1" customWidth="1"/>
+    <col min="29" max="29" width="10.8516" style="1" customWidth="1"/>
     <col min="30" max="30" width="11.1719" style="1" customWidth="1"/>
-    <col min="31" max="31" width="10.8516" style="1" customWidth="1"/>
+    <col min="31" max="31" width="11.1719" style="1" customWidth="1"/>
     <col min="32" max="32" width="10.8516" style="1" customWidth="1"/>
     <col min="33" max="33" width="10.8516" style="1" customWidth="1"/>
     <col min="34" max="34" width="10.8516" style="1" customWidth="1"/>
@@ -1495,10 +1508,11 @@
     <col min="47" max="47" width="10.8516" style="1" customWidth="1"/>
     <col min="48" max="48" width="10.8516" style="1" customWidth="1"/>
     <col min="49" max="49" width="10.8516" style="1" customWidth="1"/>
-    <col min="50" max="50" width="20.5" style="1" customWidth="1"/>
-    <col min="51" max="51" width="10.8516" style="1" customWidth="1"/>
+    <col min="50" max="50" width="10.8516" style="1" customWidth="1"/>
+    <col min="51" max="51" width="20.5" style="1" customWidth="1"/>
     <col min="52" max="52" width="10.8516" style="1" customWidth="1"/>
-    <col min="53" max="256" width="10.8516" style="1" customWidth="1"/>
+    <col min="53" max="53" width="10.8516" style="1" customWidth="1"/>
+    <col min="54" max="256" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1658,13 +1672,16 @@
       <c r="AZ1" t="s" s="2">
         <v>51</v>
       </c>
+      <c r="BA1" t="s" s="2">
+        <v>52</v>
+      </c>
     </row>
     <row r="2" ht="17" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4">
@@ -1674,106 +1691,109 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M2" s="5">
         <v>43523</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="P2" s="5">
+      <c r="N2" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="5">
         <v>45138</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="R2" s="5">
         <v>43313</v>
       </c>
-      <c r="R2" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="S2" s="5">
+      <c r="S2" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="T2" s="5">
         <v>45138</v>
       </c>
-      <c r="T2" s="5">
+      <c r="U2" s="5">
         <v>43313</v>
       </c>
-      <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
-      <c r="X2" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="5">
+      <c r="X2" s="3"/>
+      <c r="Y2" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="5">
         <v>26268</v>
       </c>
-      <c r="AA2" s="3"/>
-      <c r="AB2" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="AC2" s="4">
-        <v>7483256211</v>
+      <c r="AB2" s="3"/>
+      <c r="AC2" t="s" s="2">
+        <v>62</v>
       </c>
       <c r="AD2" s="4">
         <v>7483256211</v>
       </c>
-      <c r="AE2" t="s" s="2">
-        <v>61</v>
+      <c r="AE2" s="4">
+        <v>7483256211</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AL2" s="3"/>
-      <c r="AM2" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="AN2" s="3"/>
+      <c r="AL2" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="AM2" s="3"/>
+      <c r="AN2" t="s" s="2">
+        <v>70</v>
+      </c>
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
-      <c r="AQ2" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AR2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" t="s" s="2">
+        <v>71</v>
+      </c>
       <c r="AS2" s="3"/>
       <c r="AT2" s="3"/>
       <c r="AU2" s="3"/>
       <c r="AV2" s="3"/>
-      <c r="AW2" t="s" s="2">
-        <v>70</v>
-      </c>
+      <c r="AW2" s="3"/>
       <c r="AX2" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AY2" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AZ2" s="6">
+        <v>73</v>
+      </c>
+      <c r="AZ2" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="BA2" s="6">
         <v>38967</v>
       </c>
     </row>
@@ -1830,6 +1850,7 @@
       <c r="AX3" s="3"/>
       <c r="AY3" s="3"/>
       <c r="AZ3" s="3"/>
+      <c r="BA3" s="3"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" s="3"/>
@@ -1884,6 +1905,7 @@
       <c r="AX4" s="3"/>
       <c r="AY4" s="3"/>
       <c r="AZ4" s="3"/>
+      <c r="BA4" s="3"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" s="3"/>
@@ -1938,6 +1960,7 @@
       <c r="AX5" s="3"/>
       <c r="AY5" s="3"/>
       <c r="AZ5" s="3"/>
+      <c r="BA5" s="3"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" s="3"/>
@@ -1992,6 +2015,7 @@
       <c r="AX6" s="3"/>
       <c r="AY6" s="3"/>
       <c r="AZ6" s="3"/>
+      <c r="BA6" s="3"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" s="3"/>
@@ -2046,6 +2070,7 @@
       <c r="AX7" s="3"/>
       <c r="AY7" s="3"/>
       <c r="AZ7" s="3"/>
+      <c r="BA7" s="3"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="3"/>
@@ -2100,6 +2125,7 @@
       <c r="AX8" s="3"/>
       <c r="AY8" s="3"/>
       <c r="AZ8" s="3"/>
+      <c r="BA8" s="3"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="3"/>
@@ -2154,6 +2180,7 @@
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="3"/>
+      <c r="BA9" s="3"/>
     </row>
     <row r="10" ht="17" customHeight="1">
       <c r="A10" s="3"/>
@@ -2208,10 +2235,11 @@
       <c r="AX10" s="3"/>
       <c r="AY10" s="3"/>
       <c r="AZ10" s="3"/>
+      <c r="BA10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AB2" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="AC2" r:id="rId1" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Remove Person Status from PersonXLS processing
TISNEW-3385: Set Person Status based on ProgrammeMembership
</commit_message>
<xml_diff>
--- a/generic-upload-service/src/test/resources/TIS Recruitment Import Template - test - single.xlsx
+++ b/generic-upload-service/src/test/resources/TIS Recruitment Import Template - test - single.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
   <si>
     <t xml:space="preserve">Forenames *</t>
   </si>
@@ -43,12 +43,6 @@
     <t xml:space="preserve">Role</t>
   </si>
   <si>
-    <t xml:space="preserve">Record Status </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inactive Date</t>
-  </si>
-  <si>
     <t xml:space="preserve">Programme Name</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
   </si>
   <si>
     <t xml:space="preserve">Guy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current</t>
   </si>
   <si>
     <t xml:space="preserve">Cardiology</t>
@@ -342,7 +333,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -352,10 +343,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -392,23 +379,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BA10"/>
+  <dimension ref="A1:AY10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.7592592592593"/>
-    <col collapsed="false" hidden="false" max="13" min="2" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="42.8222222222222"/>
-    <col collapsed="false" hidden="false" max="29" min="15" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="1" width="11.4666666666667"/>
-    <col collapsed="false" hidden="false" max="50" min="32" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="1" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="256" min="52" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="11.0740740740741"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="50.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="42.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="13" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="1" width="11.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="30" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="20.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="254" min="50" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="255" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -565,131 +553,121 @@
       <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="3" t="n">
         <v>1234567</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="4" t="n">
+        <v>36218</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="4" t="n">
+        <v>45138</v>
+      </c>
+      <c r="P2" s="4" t="n">
+        <v>43313</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="R2" s="4" t="n">
+        <v>45138</v>
+      </c>
+      <c r="S2" s="4" t="n">
+        <v>43313</v>
+      </c>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="5" t="n">
-        <v>36218</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="X2" s="3"/>
+      <c r="Y2" s="4" t="n">
+        <v>26268</v>
+      </c>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q2" s="5" t="n">
-        <v>45138</v>
-      </c>
-      <c r="R2" s="5" t="n">
-        <v>43313</v>
-      </c>
-      <c r="S2" s="2" t="s">
+      <c r="AB2" s="3" t="n">
+        <v>7483256211</v>
+      </c>
+      <c r="AC2" s="3" t="n">
+        <v>7483256211</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="5" t="n">
-        <v>45138</v>
-      </c>
-      <c r="U2" s="5" t="n">
-        <v>43313</v>
-      </c>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="5" t="n">
-        <v>26268</v>
-      </c>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="6" t="s">
+      <c r="AF2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AD2" s="4" t="n">
-        <v>7483256211</v>
-      </c>
-      <c r="AE2" s="4" t="n">
-        <v>7483256211</v>
-      </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
       <c r="AQ2" s="3"/>
-      <c r="AR2" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="AR2" s="3"/>
       <c r="AS2" s="3"/>
       <c r="AT2" s="3"/>
       <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
+      <c r="AV2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="AX2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="BA2" s="7" t="n">
+        <v>71</v>
+      </c>
+      <c r="AY2" s="6" t="n">
         <v>38967</v>
       </c>
     </row>
@@ -745,8 +723,6 @@
       <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
       <c r="AY3" s="3"/>
-      <c r="AZ3" s="3"/>
-      <c r="BA3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -800,8 +776,6 @@
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
       <c r="AY4" s="3"/>
-      <c r="AZ4" s="3"/>
-      <c r="BA4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -855,8 +829,6 @@
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
       <c r="AY5" s="3"/>
-      <c r="AZ5" s="3"/>
-      <c r="BA5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
@@ -910,8 +882,6 @@
       <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
       <c r="AY6" s="3"/>
-      <c r="AZ6" s="3"/>
-      <c r="BA6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -965,8 +935,6 @@
       <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
       <c r="AY7" s="3"/>
-      <c r="AZ7" s="3"/>
-      <c r="BA7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
@@ -1020,8 +988,6 @@
       <c r="AW8" s="3"/>
       <c r="AX8" s="3"/>
       <c r="AY8" s="3"/>
-      <c r="AZ8" s="3"/>
-      <c r="BA8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -1075,8 +1041,6 @@
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
-      <c r="AZ9" s="3"/>
-      <c r="BA9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -1130,16 +1094,14 @@
       <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
       <c r="AY10" s="3"/>
-      <c r="AZ10" s="3"/>
-      <c r="BA10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AC2" r:id="rId1" display="random.guy@hotmail.co.uk"/>
+    <hyperlink ref="AA2" r:id="rId1" display="random.guy@hotmail.co.uk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;P</oddFooter>

</xml_diff>